<commit_message>
update Cmas/Etws xlsx file
</commit_message>
<xml_diff>
--- a/src/main/resources/amarisoft/cmasAndEtwsHolder.xlsx
+++ b/src/main/resources/amarisoft/cmasAndEtwsHolder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmagitsky\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sitshakov\git\Testspan_Runners\src\main\resources\amarisoft\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,9 +47,6 @@
     <t>this is a ETWS test message2</t>
   </si>
   <si>
-    <t>Earthquake warning</t>
-  </si>
-  <si>
     <t>Presidential alert</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>this is a CMAS test message6.1,this is a CMAS test message6.1, this is a CMAS test message6.1this is a CMAS test message6.2,this is a CMAS test message6.2, this is a CMAS test message6.2this is a CMAS test message6.3,this is a CMAS test message6.3, this is a CMAS test message6.3this is a CMAS test message6.4,this is a CMAS test message6.4, this is a CMAS test message6.4this is a CMAS test message6.5,this is a CMAS test message6.5, this is a CMAS test message6.5this is a CMAS test message6.6,this is a CMAS test message6.6, this is a CMAS test message6.6this is a CMAS test message6.7,this is a CMAS test message6.7, this is a CMAS test message6.7this is a CMAS test message6.8,this is a CMAS test message6.8, this is a CMAS test message6.8this is a CMAS test message6.9,this is a CMAS test message6.9, this is a CMAS test message6.9this is a CMAS test message610,this is a CMAS test message610,this is a CMAS test message6.10this is a CMAS test message611,this is a CMAS test message611,this is a CMAS test message6.11this is a CMAS test message612,this is a CMAS test message612,this is a CMAS test message6.12this is a CMAS test message613,this is a CMAS test message613,this is a CMAS test message6.13this is a CMAS test message614,this is a CMAS test message614,this is a CMAS test message6.14this is a CMAS test message615,this is a CMAS test message615,this is a CMAS test message6.15</t>
+  </si>
+  <si>
+    <t>this is a ETWS test message2,this is a ETWS test message2.1</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -437,21 +437,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -473,10 +473,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,10 +484,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,10 +495,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>